<commit_message>
fix: Modified the excel file to include more emails to enable easier testing.
</commit_message>
<xml_diff>
--- a/src/main/resources/admins.xlsx
+++ b/src/main/resources/admins.xlsx
@@ -1,20 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Srinidhi\SST\Dev\SST Internal Tools\SST-Internal-Tools-Backend\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{20476ECA-C7D3-45AD-9B3E-B47D4A3C8067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Email</t>
   </si>
@@ -29,13 +51,22 @@
   </si>
   <si>
     <t>viveksolanki@scaler.com</t>
+  </si>
+  <si>
+    <t>srinidhi.24bcs10037@sst.scaler.com</t>
+  </si>
+  <si>
+    <t>arnav.24bcs10063@sst.scaler.com</t>
+  </si>
+  <si>
+    <t>vivek.24bcs10338@sst.scaler.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +78,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,27 +123,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +192,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -176,6 +226,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -210,9 +261,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,39 +437,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{B52C5C45-26CE-43E0-8917-D2AC8A09BFA1}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{0942C073-0643-4CD5-AD5A-BC339289E31E}"/>
+    <hyperlink ref="A8" r:id="rId3" xr:uid="{B5A4482E-21D5-43C7-939D-112A682A56AB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added amrinders mail in admin list
</commit_message>
<xml_diff>
--- a/src/main/resources/admins.xlsx
+++ b/src/main/resources/admins.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Srinidhi\SST\Dev\SST Internal Tools\SST-Internal-Tools-Backend\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALA\OneDrive\Desktop\SST_Internal_Tools\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20476ECA-C7D3-45AD-9B3E-B47D4A3C8067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDC53E0-A3A9-4045-9D88-342D3F32C451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -60,6 +58,9 @@
   </si>
   <si>
     <t>vivek.24bcs10338@sst.scaler.com</t>
+  </si>
+  <si>
+    <t>amrinder.24bcs10596@sst.scaler.com</t>
   </si>
 </sst>
 </file>
@@ -438,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,11 +490,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{B52C5C45-26CE-43E0-8917-D2AC8A09BFA1}"/>
     <hyperlink ref="A7" r:id="rId2" xr:uid="{0942C073-0643-4CD5-AD5A-BC339289E31E}"/>
     <hyperlink ref="A8" r:id="rId3" xr:uid="{B5A4482E-21D5-43C7-939D-112A682A56AB}"/>
+    <hyperlink ref="A9" r:id="rId4" xr:uid="{8A1F5166-6154-4964-A59C-CDF1B9227097}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
made yash get admin privilege
</commit_message>
<xml_diff>
--- a/src/main/resources/admins.xlsx
+++ b/src/main/resources/admins.xlsx
@@ -1,92 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALA\OneDrive\Desktop\SST_Internal_Tools\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDC53E0-A3A9-4045-9D88-342D3F32C451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>arnavgupta@scaler.com</t>
-  </si>
-  <si>
-    <t>ommalviya@scaler.com</t>
-  </si>
-  <si>
-    <t>srinidhi@scaler.com</t>
-  </si>
-  <si>
-    <t>viveksolanki@scaler.com</t>
-  </si>
-  <si>
-    <t>srinidhi.24bcs10037@sst.scaler.com</t>
-  </si>
-  <si>
-    <t>arnav.24bcs10063@sst.scaler.com</t>
-  </si>
-  <si>
-    <t>vivek.24bcs10338@sst.scaler.com</t>
-  </si>
-  <si>
-    <t>amrinder.24bcs10596@sst.scaler.com</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,7 +30,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -108,54 +38,25 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,7 +94,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -265,7 +166,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -297,20 +198,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -432,76 +329,154 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet 1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>A</v>
+      </c>
+      <c r="B1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Email</v>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>arnavgupta@scaler.com</v>
+      </c>
+      <c r="B3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>ommalviya@scaler.com</v>
+      </c>
+      <c r="B4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>srinidhi@scaler.com</v>
+      </c>
+      <c r="B5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>viveksolanki@scaler.com</v>
+      </c>
+      <c r="B6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>srinidhi.24bcs10037@sst.scaler.com</v>
+      </c>
+      <c r="B7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>arnav.24bcs10063@sst.scaler.com</v>
+      </c>
+      <c r="B8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>vivek.24bcs10338@sst.scaler.com</v>
+      </c>
+      <c r="B9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>amrinder.24bcs10596@sst.scaler.com</v>
+      </c>
+      <c r="B10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>yash.24bcs10100@sst.scaler.com</v>
+      </c>
+      <c r="B11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{B52C5C45-26CE-43E0-8917-D2AC8A09BFA1}"/>
-    <hyperlink ref="A7" r:id="rId2" xr:uid="{0942C073-0643-4CD5-AD5A-BC339289E31E}"/>
-    <hyperlink ref="A8" r:id="rId3" xr:uid="{B5A4482E-21D5-43C7-939D-112A682A56AB}"/>
-    <hyperlink ref="A9" r:id="rId4" xr:uid="{8A1F5166-6154-4964-A59C-CDF1B9227097}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>